<commit_message>
Envios de correos 3
</commit_message>
<xml_diff>
--- a/plantilla.xlsx
+++ b/plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\8vo-Nivel\Sistema-CDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60273A36-21AD-46C8-BCC6-C81F7E0F7145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EFF573-2D43-4E92-83B9-4A77C30432A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Inactivo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Activo</t>
   </si>
@@ -38,9 +35,6 @@
   </si>
   <si>
     <t>johandesvos@gmail.com</t>
-  </si>
-  <si>
-    <t>`0123456789</t>
   </si>
   <si>
     <t>jdgaleas1@espe.edu.ec</t>
@@ -83,6 +77,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0000000000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -179,11 +176,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -195,13 +190,38 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000000000"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -250,9 +270,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Respuestas de formulario 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
-      <tableStyleElement type="secondRowStripe" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="secondRowStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -267,11 +287,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:G150" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:G150" headerRowDxfId="1">
   <tableColumns count="7">
     <tableColumn id="7" xr3:uid="{576D63CD-37AA-4089-BBBF-441AECBF84D4}" name="Nombres Estudiante"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Apellidos Estudiante"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Número de cédula estudiante "/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Número de cédula estudiante " dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo estudiante "/>
     <tableColumn id="5" xr3:uid="{35ACD7BE-F3C4-45BD-B20B-DF0ADED928D5}" name="Curso"/>
     <tableColumn id="1" xr3:uid="{6D5F0E06-D9E2-44F3-ADB8-E0749C3305C0}" name="Estudiante Activo/Inactivo"/>
@@ -482,18 +502,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.08984375" customWidth="1"/>
     <col min="2" max="2" width="23.90625" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" style="7" customWidth="1"/>
     <col min="4" max="4" width="24.54296875" customWidth="1"/>
     <col min="5" max="5" width="23.453125" customWidth="1"/>
     <col min="6" max="6" width="25.453125" customWidth="1"/>
@@ -502,118 +522,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="C2" s="9">
+        <v>1234567890</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="9">
+        <v>123456789</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9">
+        <v>123456789</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="26" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J26" s="1"/>
+    </row>
+    <row r="80" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -626,10 +749,12 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{9040959D-F233-4EF0-8AFF-ABD46F12C274}"/>
     <hyperlink ref="G2" r:id="rId3" xr:uid="{100061E1-5672-487C-B681-391E6C378163}"/>
     <hyperlink ref="G3" r:id="rId4" xr:uid="{332BBBAF-B7BC-4E2E-8918-BC518A16C910}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{79FF9FC3-085A-42CD-B8DA-A7FF4731F6C3}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{9F28FD1A-A9DB-40F6-B17B-AD08803C3807}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>